<commit_message>
Working Flow with Ruoya's Load Numbers
</commit_message>
<xml_diff>
--- a/ThaiModelInput.xlsx
+++ b/ThaiModelInput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williama/Library/Mobile Documents/com~apple~CloudDocs/William's Cloud/Oxford/Small Group Project/Modelling Playground/Thai-PandaPower/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850622A4-FBB7-BD4C-BB8D-FC13B42639B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EA0B49-E7A2-C441-8332-04FE81D32C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="600" windowWidth="24400" windowHeight="13720" activeTab="3" xr2:uid="{D3764318-3051-D04F-B9CB-11876FC0CA1B}"/>
+    <workbookView xWindow="11860" yWindow="500" windowWidth="24400" windowHeight="13720" activeTab="2" xr2:uid="{D3764318-3051-D04F-B9CB-11876FC0CA1B}"/>
   </bookViews>
   <sheets>
     <sheet name="buses" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
   <si>
     <t>bus_id</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>Thai is 49GW</t>
+  </si>
+  <si>
+    <t>https://iea.blob.core.windows.net/assets/dd5b10b2-b655-4c7d-8c09-d3d7efe6bd50/ThailandsCleanElectricityTransition.pdf</t>
   </si>
 </sst>
 </file>
@@ -574,7 +580,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C5"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -660,10 +666,13 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G4"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1275,11 +1284,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB71252D-3AD5-EC4D-A873-BF2AE8B3E6E0}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1315,13 +1328,13 @@
         <v>500</v>
       </c>
       <c r="D2" s="1">
-        <v>4422.4489800000001</v>
+        <v>2.19</v>
       </c>
       <c r="E2" s="1">
-        <v>2141.8897999999999</v>
+        <v>1.0606654099999999</v>
       </c>
       <c r="F2" s="1">
-        <v>4913.2641299999996</v>
+        <v>2.4333333330000002</v>
       </c>
       <c r="H2" s="1">
         <v>8.0408160000000006E-2</v>
@@ -1338,13 +1351,13 @@
         <v>230</v>
       </c>
       <c r="D3" s="1">
-        <v>6041.5816299999997</v>
+        <v>2.99</v>
       </c>
       <c r="E3" s="1">
-        <v>2926.0715300000002</v>
+        <v>1.448123093</v>
       </c>
       <c r="F3" s="1">
-        <v>6712.0924299999997</v>
+        <v>3.3222222220000002</v>
       </c>
       <c r="H3" s="1">
         <v>0.10984694</v>
@@ -1361,13 +1374,13 @@
         <v>500</v>
       </c>
       <c r="D4" s="1">
-        <v>40077.040800000002</v>
+        <v>2.21</v>
       </c>
       <c r="E4" s="1">
-        <v>19410.196800000002</v>
+        <v>1.0703518519999999</v>
       </c>
       <c r="F4" s="1">
-        <v>44524.897400000002</v>
+        <v>2.4555555560000002</v>
       </c>
       <c r="H4" s="1">
         <v>0.72867347000000005</v>
@@ -1384,13 +1397,13 @@
         <v>230</v>
       </c>
       <c r="D5" s="1">
-        <v>4461.7346900000002</v>
+        <v>19.829999999999998</v>
       </c>
       <c r="E5" s="1">
-        <v>2160.9167400000001</v>
+        <v>9.6041073390000005</v>
       </c>
       <c r="F5" s="1">
-        <v>4956.9098700000004</v>
+        <v>22.033333330000001</v>
       </c>
       <c r="H5" s="1">
         <v>8.1122449999999999E-2</v>
@@ -1468,15 +1481,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A1CB5C-C75E-D140-AAEC-4E52BCEBAC4C}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -1489,8 +1502,11 @@
       <c r="D1" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>47</v>
       </c>
@@ -1501,10 +1517,13 @@
         <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>6873.65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3939.9998400000004</v>
+      </c>
+      <c r="F2" s="1">
+        <v>8.0408160000000006E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>48</v>
       </c>
@@ -1515,10 +1534,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>7843.45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>5382.5000600000003</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.10984694</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
@@ -1529,10 +1551,13 @@
         <v>2</v>
       </c>
       <c r="D4" s="1">
-        <v>6273.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35705.000030000003</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.72867347000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>50</v>
       </c>
@@ -1543,8 +1568,51 @@
         <v>3</v>
       </c>
       <c r="D5" s="1">
-        <v>10782.58</v>
-      </c>
+        <v>3975.0000500000001</v>
+      </c>
+      <c r="F5" s="1">
+        <v>8.1122449999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10">
+        <v>49000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D11" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Thailand on background of flow
</commit_message>
<xml_diff>
--- a/ThaiModelInput.xlsx
+++ b/ThaiModelInput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williama/Library/Mobile Documents/com~apple~CloudDocs/William's Cloud/Oxford/Small Group Project/Modelling Playground/Thai-PandaPower/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EA0B49-E7A2-C441-8332-04FE81D32C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9167BE-973A-4D41-884D-5AF2A4CF7863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11860" yWindow="500" windowWidth="24400" windowHeight="13720" activeTab="2" xr2:uid="{D3764318-3051-D04F-B9CB-11876FC0CA1B}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
   <si>
     <t>bus_id</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>https://iea.blob.core.windows.net/assets/dd5b10b2-b655-4c7d-8c09-d3d7efe6bd50/ThailandsCleanElectricityTransition.pdf</t>
+  </si>
+  <si>
+    <t>Ruoya</t>
+  </si>
+  <si>
+    <t>Willi</t>
   </si>
 </sst>
 </file>
@@ -1282,10 +1288,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB71252D-3AD5-EC4D-A873-BF2AE8B3E6E0}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1327,14 +1333,14 @@
       <c r="C2" s="1">
         <v>500</v>
       </c>
-      <c r="D2" s="1">
-        <v>2.19</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1.0606654099999999</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2.4333333330000002</v>
+      <c r="D2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E2">
+        <v>2.1</v>
+      </c>
+      <c r="F2">
+        <v>4.9000000000000004</v>
       </c>
       <c r="H2" s="1">
         <v>8.0408160000000006E-2</v>
@@ -1350,14 +1356,14 @@
       <c r="C3" s="1">
         <v>230</v>
       </c>
-      <c r="D3" s="1">
-        <v>2.99</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1.448123093</v>
-      </c>
-      <c r="F3" s="1">
-        <v>3.3222222220000002</v>
+      <c r="D3">
+        <v>6.1</v>
+      </c>
+      <c r="E3">
+        <v>2.9</v>
+      </c>
+      <c r="F3">
+        <v>6.8</v>
       </c>
       <c r="H3" s="1">
         <v>0.10984694</v>
@@ -1373,14 +1379,14 @@
       <c r="C4" s="1">
         <v>500</v>
       </c>
-      <c r="D4" s="1">
-        <v>2.21</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1.0703518519999999</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2.4555555560000002</v>
+      <c r="D4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E4">
+        <v>1.9</v>
+      </c>
+      <c r="F4">
+        <v>4.5</v>
       </c>
       <c r="H4" s="1">
         <v>0.72867347000000005</v>
@@ -1396,14 +1402,14 @@
       <c r="C5" s="1">
         <v>230</v>
       </c>
-      <c r="D5" s="1">
-        <v>19.829999999999998</v>
-      </c>
-      <c r="E5" s="1">
-        <v>9.6041073390000005</v>
-      </c>
-      <c r="F5" s="1">
-        <v>22.033333330000001</v>
+      <c r="D5">
+        <v>4.5</v>
+      </c>
+      <c r="E5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F5">
+        <v>4.9000000000000004</v>
       </c>
       <c r="H5" s="1">
         <v>8.1122449999999999E-2</v>
@@ -1472,6 +1478,148 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D16" s="1">
+        <v>4422.4489800000001</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2141.8897999999999</v>
+      </c>
+      <c r="F16" s="1">
+        <v>4913.2641299999996</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D17" s="1">
+        <v>6041.5816299999997</v>
+      </c>
+      <c r="E17" s="1">
+        <v>2926.0715300000002</v>
+      </c>
+      <c r="F17" s="1">
+        <v>6712.0924299999997</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D18" s="1">
+        <v>40077.040800000002</v>
+      </c>
+      <c r="E18" s="1">
+        <v>19410.196800000002</v>
+      </c>
+      <c r="F18" s="1">
+        <v>44524.897400000002</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D19" s="1">
+        <v>4461.7346900000002</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2160.9167400000001</v>
+      </c>
+      <c r="F19" s="1">
+        <v>4956.9098700000004</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E21">
+        <v>2.1</v>
+      </c>
+      <c r="F21">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>6.1</v>
+      </c>
+      <c r="E22">
+        <v>2.9</v>
+      </c>
+      <c r="F22">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E23">
+        <v>1.9</v>
+      </c>
+      <c r="F23">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <v>4.5</v>
+      </c>
+      <c r="E24">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F24">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D28" s="1">
+        <v>2.19</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1.0606654099999999</v>
+      </c>
+      <c r="F28" s="1">
+        <v>2.43333333</v>
+      </c>
+    </row>
+    <row r="29" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D29" s="1">
+        <v>2.99</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1.4481230899999999</v>
+      </c>
+      <c r="F29" s="1">
+        <v>3.32222222</v>
+      </c>
+    </row>
+    <row r="30" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D30" s="1">
+        <v>2.21</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1.07035185</v>
+      </c>
+      <c r="F30" s="1">
+        <v>2.4555555600000001</v>
+      </c>
+    </row>
+    <row r="31" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D31" s="1">
+        <v>19.829999999999998</v>
+      </c>
+      <c r="E31" s="1">
+        <v>9.6041073400000005</v>
+      </c>
+      <c r="F31" s="1">
+        <v>22.033333299999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Hong Sa Import
</commit_message>
<xml_diff>
--- a/ThaiModelInput.xlsx
+++ b/ThaiModelInput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williama/Library/Mobile Documents/com~apple~CloudDocs/William's Cloud/Oxford/Small Group Project/Modelling Playground/Thai-PandaPower/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9167BE-973A-4D41-884D-5AF2A4CF7863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FDB20C-C500-3540-BDAF-71ADD4D53368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11860" yWindow="500" windowWidth="24400" windowHeight="13720" activeTab="2" xr2:uid="{D3764318-3051-D04F-B9CB-11876FC0CA1B}"/>
+    <workbookView xWindow="3060" yWindow="760" windowWidth="24400" windowHeight="13720" activeTab="3" xr2:uid="{D3764318-3051-D04F-B9CB-11876FC0CA1B}"/>
   </bookViews>
   <sheets>
     <sheet name="buses" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="loads" sheetId="3" r:id="rId3"/>
     <sheet name="gen" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
   <si>
     <t>bus_id</t>
   </si>
@@ -204,13 +204,40 @@
   </si>
   <si>
     <t>Willi</t>
+  </si>
+  <si>
+    <t>(102.8159, 17.3647)</t>
+  </si>
+  <si>
+    <t>(103.6520,16.0538)</t>
+  </si>
+  <si>
+    <t>(104.8473, 14)</t>
+  </si>
+  <si>
+    <t>Laos_central1</t>
+  </si>
+  <si>
+    <t>Laos_central2</t>
+  </si>
+  <si>
+    <t>Laos_south</t>
+  </si>
+  <si>
+    <t>Hong Sa</t>
+  </si>
+  <si>
+    <t></t>
+  </si>
+  <si>
+    <t>(101.583063, 19.763319)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -223,6 +250,35 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF1A73E8"/>
+      <name val="Google Symbols"/>
     </font>
   </fonts>
   <fills count="2">
@@ -242,16 +298,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{D498BBD2-4B80-C34B-8B2F-6914AE2ED033}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -583,15 +652,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C88006A-4D90-304B-84D2-9F4A420FC89B}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="4" max="4" width="21.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -605,7 +677,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -619,7 +691,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -633,7 +705,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -647,7 +719,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -659,6 +731,65 @@
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="5">
+        <v>500</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="5">
+        <v>230</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="23">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="5">
+        <v>115</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="5">
+        <v>115</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -672,15 +803,15 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="4" max="4" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -724,7 +855,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -768,7 +899,7 @@
         <v>9.5346210000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -812,7 +943,7 @@
         <v>9.5346210000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -856,24 +987,52 @@
         <v>9.5346210000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
+    <row r="5" spans="1:15">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>400</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="G5" s="1">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="1">
+        <v>2</v>
+      </c>
+      <c r="L5" s="1">
+        <v>12</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1711.4</v>
+      </c>
+      <c r="N5" s="1">
+        <v>9.5346210000000001E-2</v>
+      </c>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -890,7 +1049,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -903,7 +1062,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -916,7 +1075,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -929,7 +1088,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -942,7 +1101,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -959,7 +1118,7 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -976,7 +1135,7 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -993,7 +1152,7 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1010,7 +1169,7 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1027,7 +1186,7 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1044,7 +1203,7 @@
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1061,7 +1220,7 @@
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1078,7 +1237,7 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -1109,7 +1268,7 @@
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15">
       <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
@@ -1142,7 +1301,7 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
@@ -1171,7 +1330,7 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
@@ -1200,7 +1359,7 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15">
       <c r="A23" s="1" t="s">
         <v>40</v>
       </c>
@@ -1212,7 +1371,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1229,7 +1388,7 @@
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1246,7 +1405,7 @@
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1263,7 +1422,7 @@
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1290,17 +1449,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB71252D-3AD5-EC4D-A873-BF2AE8B3E6E0}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1323,7 +1482,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1346,7 +1505,7 @@
         <v>8.0408160000000006E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1369,7 +1528,7 @@
         <v>0.10984694</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1392,7 +1551,7 @@
         <v>0.72867347000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1415,17 +1574,29 @@
         <v>8.1122449999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+    <row r="6" spans="1:8">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="1">
+        <v>500</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-1.8</v>
+      </c>
+      <c r="E6" s="1">
+        <v>-0.87</v>
+      </c>
+      <c r="F6" s="1">
+        <v>-1.99</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1435,7 +1606,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1445,7 +1616,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1455,7 +1626,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1469,7 +1640,7 @@
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1479,7 +1650,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="D16" s="1">
         <v>4422.4489800000001</v>
       </c>
@@ -1490,7 +1661,7 @@
         <v>4913.2641299999996</v>
       </c>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:6">
       <c r="D17" s="1">
         <v>6041.5816299999997</v>
       </c>
@@ -1501,7 +1672,7 @@
         <v>6712.0924299999997</v>
       </c>
     </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:6">
       <c r="D18" s="1">
         <v>40077.040800000002</v>
       </c>
@@ -1512,7 +1683,7 @@
         <v>44524.897400000002</v>
       </c>
     </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:6">
       <c r="D19" s="1">
         <v>4461.7346900000002</v>
       </c>
@@ -1523,12 +1694,12 @@
         <v>4956.9098700000004</v>
       </c>
     </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:6">
       <c r="D20" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:6">
       <c r="D21">
         <v>4.4000000000000004</v>
       </c>
@@ -1539,7 +1710,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:6">
       <c r="D22">
         <v>6.1</v>
       </c>
@@ -1550,7 +1721,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:6">
       <c r="D23">
         <v>4.0999999999999996</v>
       </c>
@@ -1561,7 +1732,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:6">
       <c r="D24">
         <v>4.5</v>
       </c>
@@ -1572,12 +1743,12 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="4:6">
       <c r="D27" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="4:6">
       <c r="D28" s="1">
         <v>2.19</v>
       </c>
@@ -1588,7 +1759,7 @@
         <v>2.43333333</v>
       </c>
     </row>
-    <row r="29" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="4:6">
       <c r="D29" s="1">
         <v>2.99</v>
       </c>
@@ -1599,7 +1770,7 @@
         <v>3.32222222</v>
       </c>
     </row>
-    <row r="30" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="4:6">
       <c r="D30" s="1">
         <v>2.21</v>
       </c>
@@ -1610,7 +1781,7 @@
         <v>2.4555555600000001</v>
       </c>
     </row>
-    <row r="31" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="4:6">
       <c r="D31" s="1">
         <v>19.829999999999998</v>
       </c>
@@ -1631,13 +1802,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A1CB5C-C75E-D140-AAEC-4E52BCEBAC4C}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -1654,7 +1825,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>47</v>
       </c>
@@ -1671,7 +1842,7 @@
         <v>8.0408160000000006E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>48</v>
       </c>
@@ -1688,7 +1859,7 @@
         <v>0.10984694</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
@@ -1705,7 +1876,7 @@
         <v>0.72867347000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>50</v>
       </c>
@@ -1722,19 +1893,19 @@
         <v>8.1122449999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="D10" s="1" t="s">
         <v>51</v>
       </c>
@@ -1742,24 +1913,24 @@
         <v>49000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="D11" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="D16" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Raise kA for Bangkok to Northeast
</commit_message>
<xml_diff>
--- a/ThaiModelInput.xlsx
+++ b/ThaiModelInput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williama/Library/Mobile Documents/com~apple~CloudDocs/William's Cloud/Oxford/Small Group Project/Modelling Playground/Thai-PandaPower/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6768B2-E893-FE4C-BA27-6E092971BC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFE986B-5694-714D-B428-3B1F42CF41AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="760" windowWidth="24400" windowHeight="13720" activeTab="2" xr2:uid="{D3764318-3051-D04F-B9CB-11876FC0CA1B}"/>
+    <workbookView xWindow="3060" yWindow="760" windowWidth="24400" windowHeight="13720" activeTab="1" xr2:uid="{D3764318-3051-D04F-B9CB-11876FC0CA1B}"/>
   </bookViews>
   <sheets>
     <sheet name="buses" sheetId="1" r:id="rId1"/>
@@ -689,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C88006A-4D90-304B-84D2-9F4A420FC89B}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:C11"/>
+    <sheetView zoomScale="138" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -871,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F51210-D4A9-FA40-ABBE-75E4FA51A6A8}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -944,7 +944,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G2" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H2" s="1">
         <v>3</v>
@@ -988,7 +988,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G3" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H3" s="1">
         <v>3</v>
@@ -1670,8 +1670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB71252D-3AD5-EC4D-A873-BF2AE8B3E6E0}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView zoomScale="136" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2122,7 +2122,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Preparing for 2050 inputs
</commit_message>
<xml_diff>
--- a/ThaiModelInput.xlsx
+++ b/ThaiModelInput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williama/Library/Mobile Documents/com~apple~CloudDocs/William's Cloud/Oxford/Small Group Project/Modelling Playground/Thai-PandaPower/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFE986B-5694-714D-B428-3B1F42CF41AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F794D75-D42A-4B47-8356-9A60FFB0E8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="760" windowWidth="24400" windowHeight="13720" activeTab="1" xr2:uid="{D3764318-3051-D04F-B9CB-11876FC0CA1B}"/>
+    <workbookView xWindow="3060" yWindow="760" windowWidth="24400" windowHeight="13720" activeTab="2" xr2:uid="{D3764318-3051-D04F-B9CB-11876FC0CA1B}"/>
   </bookViews>
   <sheets>
     <sheet name="buses" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="79">
   <si>
     <t>bus_id</t>
   </si>
@@ -206,24 +206,15 @@
     <t>Willi</t>
   </si>
   <si>
-    <t>Hong Sa</t>
-  </si>
-  <si>
     <t>(101.583063, 19.763319)</t>
   </si>
   <si>
-    <t>Nam Ngum</t>
-  </si>
-  <si>
     <t>https://www.ceicdata.com/en/thailand/electricity-statistics/electricity-peak-demand-net</t>
   </si>
   <si>
     <t>102.547381, 18.483688</t>
   </si>
   <si>
-    <t>Theun-Hinboun</t>
-  </si>
-  <si>
     <t></t>
   </si>
   <si>
@@ -233,22 +224,58 @@
     <t>https://www.worldbank.org/en/country/lao/brief/nam-theun-2-project-overview-and-update</t>
   </si>
   <si>
-    <t>Houay Ho</t>
-  </si>
-  <si>
     <t>106.760822, 15.059154</t>
   </si>
   <si>
-    <t>Cambodia Export</t>
-  </si>
-  <si>
     <t>103.812983, 13.254713</t>
   </si>
   <si>
-    <t>Malaysia Export</t>
-  </si>
-  <si>
     <t>100.549331, 5.806423</t>
+  </si>
+  <si>
+    <t>Thailand-North</t>
+  </si>
+  <si>
+    <t>Thailand-Northeast</t>
+  </si>
+  <si>
+    <t>Thailand-Bangkok</t>
+  </si>
+  <si>
+    <t>Thailand-South</t>
+  </si>
+  <si>
+    <t>Import-Laos-Nam Ngum</t>
+  </si>
+  <si>
+    <t>Import-Laos-Theun-Hinboun</t>
+  </si>
+  <si>
+    <t>Import-Laos-Houay Ho</t>
+  </si>
+  <si>
+    <t>Export-Cambodia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Export-Malaysia </t>
+  </si>
+  <si>
+    <t>Import-Laos-Hong Sa</t>
+  </si>
+  <si>
+    <t>Peak Power</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>p_mw_2050</t>
+  </si>
+  <si>
+    <t>power_p_mw_2050</t>
+  </si>
+  <si>
+    <t>power_q_mvar_2050</t>
   </si>
 </sst>
 </file>
@@ -690,7 +717,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScale="138" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -717,7 +744,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="C2" s="1">
         <v>500</v>
@@ -731,7 +758,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="C3" s="1">
         <v>230</v>
@@ -745,7 +772,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="C4" s="1">
         <v>500</v>
@@ -759,7 +786,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="C5" s="1">
         <v>230</v>
@@ -773,13 +800,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="C6" s="5">
         <v>500</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -787,13 +814,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="C7" s="5">
         <v>115</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -801,13 +828,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C8" s="5">
         <v>230</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="7"/>
@@ -817,16 +844,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C9" s="5">
         <v>230</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -834,13 +861,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C10" s="12">
         <v>115</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -848,13 +875,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C11" s="12">
         <v>300</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F11" s="7"/>
     </row>
@@ -871,7 +898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F51210-D4A9-FA40-ABBE-75E4FA51A6A8}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -1668,10 +1695,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB71252D-3AD5-EC4D-A873-BF2AE8B3E6E0}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView zoomScale="136" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1680,7 +1707,7 @@
     <col min="5" max="5" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1699,22 +1726,28 @@
       <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="H1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="C2" s="1">
         <v>500</v>
       </c>
       <c r="D2" s="1">
-        <f>H2*$D$15</f>
+        <f>J2*$D$15</f>
         <v>2171.0203200000001</v>
       </c>
       <c r="E2" s="1">
@@ -1725,22 +1758,22 @@
         <f>D2*$G$13</f>
         <v>2411.9659300276512</v>
       </c>
-      <c r="H2" s="1">
+      <c r="J2" s="1">
         <v>8.0408160000000006E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="C3" s="1">
         <v>230</v>
       </c>
       <c r="D3" s="1">
-        <f>H3*$D$15</f>
+        <f>J3*$D$15</f>
         <v>2965.8673800000001</v>
       </c>
       <c r="E3" s="1">
@@ -1751,22 +1784,22 @@
         <f>D3*$G$13</f>
         <v>3295.0272310396308</v>
       </c>
-      <c r="H3" s="1">
+      <c r="J3" s="1">
         <v>0.10984694</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="C4" s="1">
         <v>500</v>
       </c>
       <c r="D4" s="1">
-        <f>H4*$D$15</f>
+        <f>J4*$D$15</f>
         <v>19674.183690000002</v>
       </c>
       <c r="E4" s="1">
@@ -1777,22 +1810,22 @@
         <f>D4*$G$13</f>
         <v>21857.676929244815</v>
       </c>
-      <c r="H4" s="1">
+      <c r="J4" s="1">
         <v>0.72867347000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="C5" s="1">
         <v>230</v>
       </c>
       <c r="D5" s="1">
-        <f>H5*$D$15</f>
+        <f>J5*$D$15</f>
         <v>2190.3061499999999</v>
       </c>
       <c r="E5" s="1">
@@ -1803,16 +1836,16 @@
         <f>D5*$G$13</f>
         <v>2433.3921527413586</v>
       </c>
-      <c r="H5" s="1">
+      <c r="J5" s="1">
         <v>8.1122449999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="C6" s="1">
         <v>500</v>
@@ -1831,12 +1864,12 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="C7" s="5">
         <v>115</v>
@@ -1855,12 +1888,12 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C8" s="5">
         <v>230</v>
@@ -1879,15 +1912,15 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C9" s="1">
         <v>230</v>
@@ -1906,12 +1939,12 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" s="10">
         <v>8</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C10" s="12">
         <v>115</v>
@@ -1929,12 +1962,12 @@
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" s="10">
         <v>9</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C11" s="12">
         <v>300</v>
@@ -1953,7 +1986,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="F13" s="1">
         <v>0.48457143000000003</v>
       </c>
@@ -1961,15 +1994,15 @@
         <v>1.1109826599999999</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="D15" s="8">
         <v>27000</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="D16" s="1">
         <v>4422.4489800000001</v>
       </c>
@@ -1980,7 +2013,7 @@
         <v>4913.2641299999996</v>
       </c>
     </row>
-    <row r="17" spans="4:6">
+    <row r="17" spans="4:10">
       <c r="D17" s="1">
         <v>6041.5816299999997</v>
       </c>
@@ -1990,8 +2023,11 @@
       <c r="F17" s="1">
         <v>6712.0924299999997</v>
       </c>
-    </row>
-    <row r="18" spans="4:6">
+      <c r="I17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10">
       <c r="D18" s="1">
         <v>40077.040800000002</v>
       </c>
@@ -2001,8 +2037,14 @@
       <c r="F18" s="1">
         <v>44524.897400000002</v>
       </c>
-    </row>
-    <row r="19" spans="4:6">
+      <c r="I18" t="s">
+        <v>75</v>
+      </c>
+      <c r="J18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10">
       <c r="D19" s="1">
         <v>4461.7346900000002</v>
       </c>
@@ -2013,12 +2055,12 @@
         <v>4956.9098700000004</v>
       </c>
     </row>
-    <row r="20" spans="4:6">
+    <row r="20" spans="4:10">
       <c r="D20" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="4:6">
+    <row r="21" spans="4:10">
       <c r="D21">
         <v>4.4000000000000004</v>
       </c>
@@ -2029,7 +2071,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="22" spans="4:6">
+    <row r="22" spans="4:10">
       <c r="D22">
         <v>6.1</v>
       </c>
@@ -2040,7 +2082,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="23" spans="4:6">
+    <row r="23" spans="4:10">
       <c r="D23">
         <v>4.0999999999999996</v>
       </c>
@@ -2051,7 +2093,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="24" spans="4:6">
+    <row r="24" spans="4:10">
       <c r="D24">
         <v>4.5</v>
       </c>
@@ -2062,12 +2104,12 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="27" spans="4:6">
+    <row r="27" spans="4:10">
       <c r="D27" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="4:6">
+    <row r="28" spans="4:10">
       <c r="D28" s="1">
         <v>2.19</v>
       </c>
@@ -2078,7 +2120,7 @@
         <v>2.43333333</v>
       </c>
     </row>
-    <row r="29" spans="4:6">
+    <row r="29" spans="4:10">
       <c r="D29" s="1">
         <v>2.99</v>
       </c>
@@ -2089,7 +2131,7 @@
         <v>3.32222222</v>
       </c>
     </row>
-    <row r="30" spans="4:6">
+    <row r="30" spans="4:10">
       <c r="D30" s="1">
         <v>2.21</v>
       </c>
@@ -2100,7 +2142,7 @@
         <v>2.4555555600000001</v>
       </c>
     </row>
-    <row r="31" spans="4:6">
+    <row r="31" spans="4:10">
       <c r="D31" s="1">
         <v>19.829999999999998</v>
       </c>
@@ -2122,7 +2164,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2140,6 +2182,9 @@
       <c r="D1" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="F1" s="1" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Added dbase and 2050 figures
</commit_message>
<xml_diff>
--- a/ThaiModelInput.xlsx
+++ b/ThaiModelInput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williama/Library/Mobile Documents/com~apple~CloudDocs/William's Cloud/Oxford/Small Group Project/Modelling Playground/Thai-PandaPower/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F794D75-D42A-4B47-8356-9A60FFB0E8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B90F5ED-5172-664C-A1F0-875C70CD22E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="760" windowWidth="24400" windowHeight="13720" activeTab="2" xr2:uid="{D3764318-3051-D04F-B9CB-11876FC0CA1B}"/>
+    <workbookView xWindow="3060" yWindow="760" windowWidth="24400" windowHeight="13720" activeTab="3" xr2:uid="{D3764318-3051-D04F-B9CB-11876FC0CA1B}"/>
   </bookViews>
   <sheets>
     <sheet name="buses" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
   <si>
     <t>bus_id</t>
   </si>
@@ -53,27 +53,15 @@
     <t>geodata</t>
   </si>
   <si>
-    <t>North</t>
-  </si>
-  <si>
     <t>(99.465678, 17.876223)</t>
   </si>
   <si>
-    <t>Northeast</t>
-  </si>
-  <si>
     <t>(103.376811, 16.659276)</t>
   </si>
   <si>
-    <t>Bangkok</t>
-  </si>
-  <si>
     <t>(100.516049, 13.687099)</t>
   </si>
   <si>
-    <t>South</t>
-  </si>
-  <si>
     <t>(99.509623, 8.104839)</t>
   </si>
   <si>
@@ -200,12 +188,6 @@
     <t>https://iea.blob.core.windows.net/assets/dd5b10b2-b655-4c7d-8c09-d3d7efe6bd50/ThailandsCleanElectricityTransition.pdf</t>
   </si>
   <si>
-    <t>Ruoya</t>
-  </si>
-  <si>
-    <t>Willi</t>
-  </si>
-  <si>
     <t>(101.583063, 19.763319)</t>
   </si>
   <si>
@@ -263,12 +245,6 @@
     <t>Import-Laos-Hong Sa</t>
   </si>
   <si>
-    <t>Peak Power</t>
-  </si>
-  <si>
-    <t>Energy</t>
-  </si>
-  <si>
     <t>p_mw_2050</t>
   </si>
   <si>
@@ -276,6 +252,48 @@
   </si>
   <si>
     <t>power_q_mvar_2050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculated Power demand (MW) using </t>
+  </si>
+  <si>
+    <t>300GW</t>
+  </si>
+  <si>
+    <t>Generation</t>
+  </si>
+  <si>
+    <t>Now</t>
+  </si>
+  <si>
+    <t>Future</t>
+  </si>
+  <si>
+    <t>(From Model)</t>
+  </si>
+  <si>
+    <t>Now Load</t>
+  </si>
+  <si>
+    <t>Future Load</t>
+  </si>
+  <si>
+    <t>Now Generation</t>
+  </si>
+  <si>
+    <t>Future Generation</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>vn_kv_2050</t>
+  </si>
+  <si>
+    <t>https://www.pwc.com/sg/en/publications/regional-electricity-trade-in-asean.html</t>
+  </si>
+  <si>
+    <t>Interconnections</t>
   </si>
 </sst>
 </file>
@@ -353,7 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -370,15 +388,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,14 +723,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C88006A-4D90-304B-84D2-9F4A420FC89B}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView zoomScale="138" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B11"/>
+    <sheetView topLeftCell="A6" zoomScale="138" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="2" max="2" width="23" customWidth="1"/>
     <col min="4" max="4" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -736,6 +746,9 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -744,13 +757,17 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1">
         <v>500</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
+      <c r="D2">
+        <f>2.5*C2</f>
+        <v>1250</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -758,13 +775,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C3" s="1">
         <v>230</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
+      <c r="D3">
+        <f t="shared" ref="D3:D5" si="0">2.5*C3</f>
+        <v>575</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -772,13 +793,17 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C4" s="1">
         <v>500</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1250</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -786,13 +811,17 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C5" s="1">
         <v>230</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>575</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -800,13 +829,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C6" s="5">
         <v>500</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>55</v>
+      <c r="D6">
+        <v>500</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -814,13 +846,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C7" s="5">
         <v>115</v>
       </c>
-      <c r="D7" t="s">
-        <v>57</v>
+      <c r="D7">
+        <v>115</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -828,13 +863,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C8" s="5">
         <v>230</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>59</v>
+      <c r="D8">
+        <v>230</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="7"/>
@@ -844,49 +882,68 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C9" s="5">
         <v>230</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>61</v>
+      <c r="D9">
+        <v>230</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="10">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="12">
+      <c r="B10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="5">
         <v>115</v>
       </c>
-      <c r="D10" t="s">
-        <v>62</v>
+      <c r="D10">
+        <v>115</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="10">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="12">
+      <c r="B11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="5">
         <v>300</v>
       </c>
-      <c r="D11" t="s">
-        <v>63</v>
+      <c r="D11">
+        <v>300</v>
+      </c>
+      <c r="E11" t="s">
+        <v>57</v>
       </c>
       <c r="F11" s="7"/>
     </row>
     <row r="13" spans="1:7">
       <c r="D13" s="7"/>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -898,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F51210-D4A9-FA40-ABBE-75E4FA51A6A8}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView zoomScale="140" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -909,46 +966,46 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -959,7 +1016,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="D2" s="1">
         <v>0.01</v>
@@ -977,10 +1034,10 @@
         <v>3</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K2" s="1">
         <v>2</v>
@@ -1003,7 +1060,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="D3" s="1">
         <v>0.01</v>
@@ -1021,10 +1078,10 @@
         <v>3</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K3" s="1">
         <v>2</v>
@@ -1047,7 +1104,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="D4" s="1">
         <v>0.01</v>
@@ -1065,10 +1122,10 @@
         <v>3</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K4" s="1">
         <v>2</v>
@@ -1091,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="D5" s="1">
         <v>0.01</v>
@@ -1109,10 +1166,10 @@
         <v>3</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K5" s="1">
         <v>2</v>
@@ -1136,7 +1193,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="D6" s="1">
         <v>0.01</v>
@@ -1154,10 +1211,10 @@
         <v>3</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K6" s="1">
         <v>2</v>
@@ -1181,7 +1238,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="D7" s="1">
         <v>0.01</v>
@@ -1199,10 +1256,10 @@
         <v>3</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K7" s="1">
         <v>2</v>
@@ -1225,7 +1282,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="D8" s="1">
         <v>0.01</v>
@@ -1243,10 +1300,10 @@
         <v>3</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K8" s="1">
         <v>2</v>
@@ -1269,7 +1326,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="1">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="D9" s="1">
         <v>0.01</v>
@@ -1287,10 +1344,10 @@
         <v>3</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K9" s="1">
         <v>2</v>
@@ -1331,10 +1388,10 @@
         <v>3</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K10" s="1">
         <v>2</v>
@@ -1427,7 +1484,9 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="J15" s="1">
+        <v>40</v>
+      </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -1444,7 +1503,9 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="J16" s="1">
+        <v>30</v>
+      </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -1461,7 +1522,9 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="J17" s="1">
+        <v>20</v>
+      </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -1470,7 +1533,7 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1480,36 +1543,40 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
+      <c r="J18" s="1">
+        <v>20</v>
+      </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="H19" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
+      <c r="J19" s="1">
+        <v>20</v>
+      </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -1518,13 +1585,13 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D20" s="1">
         <v>306.10000000000002</v>
@@ -1533,7 +1600,7 @@
         <v>9.5469999999999999E-2</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G20" s="2">
         <v>1.0000000000000001E-9</v>
@@ -1542,7 +1609,9 @@
         <v>0.83</v>
       </c>
       <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
+      <c r="J20" s="1">
+        <v>20</v>
+      </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -1553,7 +1622,7 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D21" s="1">
         <v>170.2</v>
@@ -1562,7 +1631,7 @@
         <v>0.17169999999999999</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G21" s="2">
         <v>1.0000000000000001E-9</v>
@@ -1571,7 +1640,9 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
+      <c r="J21" s="1">
+        <v>20</v>
+      </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -1582,7 +1653,7 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D22" s="1">
         <v>1711.4</v>
@@ -1591,7 +1662,7 @@
         <v>2.8379999999999999E-2</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G22" s="2">
         <v>1</v>
@@ -1600,7 +1671,9 @@
         <v>1.875</v>
       </c>
       <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
+      <c r="J22" s="1">
+        <v>20</v>
+      </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -1609,7 +1682,7 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1618,6 +1691,9 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
+      <c r="J23" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="24" spans="1:15">
       <c r="A24" s="1"/>
@@ -1697,14 +1773,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB71252D-3AD5-EC4D-A873-BF2AE8B3E6E0}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView zoomScale="136" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1718,22 +1796,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1741,22 +1819,30 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1">
         <v>500</v>
       </c>
       <c r="D2" s="1">
-        <f>J2*$D$15</f>
+        <f>J2*$B$19</f>
         <v>2171.0203200000001</v>
       </c>
       <c r="E2" s="1">
-        <f>D2*$F$13</f>
+        <f t="shared" ref="E2:E11" si="0">D2*$C$13</f>
         <v>1052.0144210214578</v>
       </c>
       <c r="F2" s="1">
-        <f>D2*$G$13</f>
+        <f t="shared" ref="F2:F11" si="1">D2*$D$13</f>
         <v>2411.9659300276512</v>
+      </c>
+      <c r="G2">
+        <f>J2*$C$24</f>
+        <v>13291.961142857144</v>
+      </c>
+      <c r="H2">
+        <f>G2*$C$13</f>
+        <v>6440.904618498721</v>
       </c>
       <c r="J2" s="1">
         <v>8.0408160000000006E-2</v>
@@ -1767,22 +1853,30 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C3" s="1">
         <v>230</v>
       </c>
       <c r="D3" s="1">
-        <f>J3*$D$15</f>
+        <f>J3*$B$19</f>
         <v>2965.8673800000001</v>
       </c>
       <c r="E3" s="1">
-        <f>D3*$F$13</f>
+        <f t="shared" si="0"/>
         <v>1437.1745975169536</v>
       </c>
       <c r="F3" s="1">
-        <f>D3*$G$13</f>
+        <f t="shared" si="1"/>
         <v>3295.0272310396308</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G5" si="2">J3*$C$24</f>
+        <v>18158.371714285713</v>
+      </c>
+      <c r="H3">
+        <f>G3*$C$13</f>
+        <v>8799.0281480629801</v>
       </c>
       <c r="J3" s="1">
         <v>0.10984694</v>
@@ -1793,22 +1887,30 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C4" s="1">
         <v>500</v>
       </c>
       <c r="D4" s="1">
-        <f>J4*$D$15</f>
+        <f>J4*$B$19</f>
         <v>19674.183690000002</v>
       </c>
       <c r="E4" s="1">
-        <f>D4*$F$13</f>
+        <f t="shared" si="0"/>
         <v>9533.5473247459777</v>
       </c>
       <c r="F4" s="1">
-        <f>D4*$G$13</f>
+        <f t="shared" si="1"/>
         <v>21857.676929244815</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>120454.18585714286</v>
+      </c>
+      <c r="H4">
+        <f>G4*$C$13</f>
+        <v>58368.657090281493</v>
       </c>
       <c r="J4" s="1">
         <v>0.72867347000000005</v>
@@ -1819,22 +1921,30 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C5" s="1">
         <v>230</v>
       </c>
       <c r="D5" s="1">
-        <f>J5*$D$15</f>
+        <f>J5*$B$19</f>
         <v>2190.3061499999999</v>
       </c>
       <c r="E5" s="1">
-        <f>D5*$F$13</f>
+        <f t="shared" si="0"/>
         <v>1061.3597832432945</v>
       </c>
       <c r="F5" s="1">
-        <f>D5*$G$13</f>
+        <f t="shared" si="1"/>
         <v>2433.3921527413586</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>13410.037653061223</v>
+      </c>
+      <c r="H5">
+        <f>G5*$C$13</f>
+        <v>6498.1211218977214</v>
       </c>
       <c r="J5" s="1">
         <v>8.1122449999999999E-2</v>
@@ -1845,7 +1955,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C6" s="1">
         <v>500</v>
@@ -1854,22 +1964,26 @@
         <v>-1473</v>
       </c>
       <c r="E6" s="1">
-        <f>D6*$F$13</f>
+        <f t="shared" si="0"/>
         <v>-713.77371639</v>
       </c>
       <c r="F6" s="1">
-        <f>D6*$G$13</f>
+        <f t="shared" si="1"/>
         <v>-1636.4774581799998</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="G6" s="1">
+        <v>-1473</v>
+      </c>
+      <c r="H6">
+        <v>-713.77371639</v>
+      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C7" s="5">
         <v>115</v>
@@ -1878,22 +1992,26 @@
         <v>-150</v>
       </c>
       <c r="E7" s="1">
-        <f>D7*$F$13</f>
+        <f t="shared" si="0"/>
         <v>-72.685714500000003</v>
       </c>
       <c r="F7" s="1">
-        <f>D7*$G$13</f>
+        <f t="shared" si="1"/>
         <v>-166.64739899999998</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="G7" s="1">
+        <v>-150</v>
+      </c>
+      <c r="H7">
+        <v>-72.685714500000003</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C8" s="5">
         <v>230</v>
@@ -1902,17 +2020,21 @@
         <v>-1000</v>
       </c>
       <c r="E8" s="1">
-        <f>D8*$F$13</f>
+        <f t="shared" si="0"/>
         <v>-484.57143000000002</v>
       </c>
       <c r="F8" s="1">
-        <f>D8*$G$13</f>
+        <f t="shared" si="1"/>
         <v>-1110.9826599999999</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="G8" s="1">
+        <v>-1000</v>
+      </c>
+      <c r="H8">
+        <v>-484.57143000000002</v>
+      </c>
       <c r="I8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1920,7 +2042,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C9" s="1">
         <v>230</v>
@@ -1929,229 +2051,170 @@
         <v>-150</v>
       </c>
       <c r="E9" s="1">
-        <f>D9*$F$13</f>
+        <f t="shared" si="0"/>
         <v>-72.685714500000003</v>
       </c>
       <c r="F9" s="1">
-        <f>D9*$G$13</f>
+        <f t="shared" si="1"/>
         <v>-166.64739899999998</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="G9" s="1">
+        <v>-150</v>
+      </c>
+      <c r="H9">
+        <v>-72.685714500000003</v>
+      </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="10">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="12">
+      <c r="B10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="5">
         <v>115</v>
       </c>
       <c r="D10" s="1">
         <v>135.5</v>
       </c>
       <c r="E10" s="1">
-        <f>D10*$F$13</f>
+        <f t="shared" si="0"/>
         <v>65.659428765000001</v>
       </c>
       <c r="F10" s="1">
-        <f>D10*$G$13</f>
+        <f t="shared" si="1"/>
         <v>150.53815042999997</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="G10" s="1">
+        <v>135.5</v>
+      </c>
+      <c r="H10">
+        <v>65.659428765000001</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="10">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="12">
+      <c r="B11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="5">
         <v>300</v>
       </c>
       <c r="D11" s="1">
         <v>100</v>
       </c>
       <c r="E11" s="1">
-        <f>D11*$F$13</f>
+        <f t="shared" si="0"/>
         <v>48.457143000000002</v>
       </c>
       <c r="F11" s="1">
-        <f>D11*$G$13</f>
+        <f t="shared" si="1"/>
         <v>111.098266</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="G11" s="1">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>48.457143000000002</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="F13" s="1">
+      <c r="C13" s="1">
         <v>0.48457143000000003</v>
       </c>
-      <c r="G13" s="1">
+      <c r="D13" s="1">
         <v>1.1109826599999999</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
-      <c r="D15" s="8">
+    <row r="16" spans="1:10">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="8">
         <v>27000</v>
       </c>
-      <c r="E15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="D16" s="1">
-        <v>4422.4489800000001</v>
-      </c>
-      <c r="E16" s="1">
-        <v>2141.8897999999999</v>
-      </c>
-      <c r="F16" s="1">
-        <v>4913.2641299999996</v>
-      </c>
-    </row>
-    <row r="17" spans="4:10">
-      <c r="D17" s="1">
-        <v>6041.5816299999997</v>
-      </c>
-      <c r="E17" s="1">
-        <v>2926.0715300000002</v>
-      </c>
-      <c r="F17" s="1">
-        <v>6712.0924299999997</v>
-      </c>
-      <c r="I17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="4:10">
-      <c r="D18" s="1">
-        <v>40077.040800000002</v>
-      </c>
-      <c r="E18" s="1">
-        <v>19410.196800000002</v>
-      </c>
-      <c r="F18" s="1">
-        <v>44524.897400000002</v>
-      </c>
-      <c r="I18" t="s">
-        <v>75</v>
-      </c>
-      <c r="J18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="4:10">
-      <c r="D19" s="1">
-        <v>4461.7346900000002</v>
-      </c>
-      <c r="E19" s="1">
-        <v>2160.9167400000001</v>
-      </c>
-      <c r="F19" s="1">
-        <v>4956.9098700000004</v>
-      </c>
-    </row>
-    <row r="20" spans="4:10">
-      <c r="D20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="4:10">
-      <c r="D21">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E21">
-        <v>2.1</v>
-      </c>
-      <c r="F21">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="22" spans="4:10">
-      <c r="D22">
-        <v>6.1</v>
-      </c>
-      <c r="E22">
-        <v>2.9</v>
-      </c>
-      <c r="F22">
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="23" spans="4:10">
-      <c r="D23">
-        <v>4.0999999999999996</v>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="F22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23">
+        <v>27000</v>
+      </c>
+      <c r="D23" t="s">
+        <v>79</v>
       </c>
       <c r="E23">
-        <v>1.9</v>
+        <v>49000</v>
       </c>
       <c r="F23">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="24" spans="4:10">
-      <c r="D24">
-        <v>4.5</v>
+        <f>E24/E23</f>
+        <v>6.1224489795918364</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24">
+        <f>(C23/E23)*E24</f>
+        <v>165306.12244897959</v>
+      </c>
+      <c r="D24" t="s">
+        <v>80</v>
       </c>
       <c r="E24">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F24">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="27" spans="4:10">
-      <c r="D27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="4:10">
-      <c r="D28" s="1">
-        <v>2.19</v>
-      </c>
-      <c r="E28" s="1">
-        <v>1.0606654099999999</v>
-      </c>
-      <c r="F28" s="1">
-        <v>2.43333333</v>
-      </c>
-    </row>
-    <row r="29" spans="4:10">
-      <c r="D29" s="1">
-        <v>2.99</v>
-      </c>
-      <c r="E29" s="1">
-        <v>1.4481230899999999</v>
-      </c>
-      <c r="F29" s="1">
-        <v>3.32222222</v>
-      </c>
-    </row>
-    <row r="30" spans="4:10">
-      <c r="D30" s="1">
-        <v>2.21</v>
-      </c>
-      <c r="E30" s="1">
-        <v>1.07035185</v>
-      </c>
-      <c r="F30" s="1">
-        <v>2.4555555600000001</v>
-      </c>
-    </row>
-    <row r="31" spans="4:10">
-      <c r="D31" s="1">
-        <v>19.829999999999998</v>
-      </c>
-      <c r="E31" s="1">
-        <v>9.6041073400000005</v>
-      </c>
-      <c r="F31" s="1">
-        <v>22.033333299999999</v>
-      </c>
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2163,15 +2226,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A1CB5C-C75E-D140-AAEC-4E52BCEBAC4C}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2180,21 +2246,21 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -2202,16 +2268,20 @@
       <c r="D2" s="1">
         <v>3939.9998400000004</v>
       </c>
+      <c r="E2">
+        <f>F2*$E$13</f>
+        <v>24122.448</v>
+      </c>
       <c r="F2" s="1">
         <v>8.0408160000000006E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -2219,16 +2289,20 @@
       <c r="D3" s="1">
         <v>5382.5000600000003</v>
       </c>
+      <c r="E3">
+        <f>F3*$E$13</f>
+        <v>32954.082000000002</v>
+      </c>
       <c r="F3" s="1">
         <v>0.10984694</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -2236,16 +2310,20 @@
       <c r="D4" s="1">
         <v>35705.000030000003</v>
       </c>
+      <c r="E4">
+        <f>F4*$E$13</f>
+        <v>218602.04100000003</v>
+      </c>
       <c r="F4" s="1">
         <v>0.72867347000000005</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -2253,6 +2331,10 @@
       <c r="D5" s="1">
         <v>3975.0000500000001</v>
       </c>
+      <c r="E5">
+        <f>F5*$E$13</f>
+        <v>24336.735000000001</v>
+      </c>
       <c r="F5" s="1">
         <v>8.1122449999999999E-2</v>
       </c>
@@ -2267,6 +2349,12 @@
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:6">
+      <c r="B9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
       <c r="D9" s="1">
         <f>SUM(D2:D5)</f>
         <v>49002.499980000008</v>
@@ -2274,7 +2362,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="D10" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E10">
         <v>49000</v>
@@ -2282,17 +2370,27 @@
     </row>
     <row r="11" spans="1:6">
       <c r="D11" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="D12" s="1"/>
+        <v>48</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="D13" s="1"/>
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13">
+        <v>300000</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="D14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
       <c r="D15" s="1"/>

</xml_diff>

<commit_message>
Convergence by adding new lines
</commit_message>
<xml_diff>
--- a/ThaiModelInput.xlsx
+++ b/ThaiModelInput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Royal\GitHub\Thai-PandaPower\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williama/Library/Mobile Documents/com~apple~CloudDocs/William's Cloud/Oxford/Small Group Project/Modelling Playground/Thai-PandaPower/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6C2297-C66B-45C8-9AB0-7A021140EA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E00033-CA78-6E43-949A-C14ACDD6F9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" activeTab="3" xr2:uid="{D3764318-3051-D04F-B9CB-11876FC0CA1B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="26200" windowHeight="16640" xr2:uid="{D3764318-3051-D04F-B9CB-11876FC0CA1B}"/>
   </bookViews>
   <sheets>
     <sheet name="buses" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="96">
   <si>
     <t>bus_id</t>
   </si>
@@ -332,6 +332,9 @@
   <si>
     <t>230 GW</t>
     <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2050 Voltage Factor</t>
   </si>
 </sst>
 </file>
@@ -342,14 +345,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -395,7 +398,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -403,7 +406,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -453,8 +456,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{D498BBD2-4B80-C34B-8B2F-6914AE2ED033}"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -470,7 +473,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -786,19 +789,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C88006A-4D90-304B-84D2-9F4A420FC89B}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="138" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="4" max="4" width="21.84375" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -815,7 +818,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -826,14 +829,17 @@
         <v>500</v>
       </c>
       <c r="D2">
-        <f>2.5*C2</f>
-        <v>1250</v>
+        <f>C2*$I$3</f>
+        <v>500</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="I2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -844,14 +850,17 @@
         <v>230</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D5" si="0">2.5*C3</f>
-        <v>575</v>
+        <f t="shared" ref="D3:D5" si="0">C3*$I$3</f>
+        <v>230</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -863,13 +872,13 @@
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>1250</v>
+        <v>500</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -881,13 +890,13 @@
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>575</v>
+        <v>230</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -904,7 +913,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -921,7 +930,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -940,7 +949,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:7" ht="22.5">
+    <row r="9" spans="1:9" ht="23">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -960,7 +969,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:9">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -977,7 +986,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:9">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -995,7 +1004,7 @@
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:9">
       <c r="D13" s="7"/>
     </row>
     <row r="17" spans="2:2">
@@ -1017,15 +1026,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F51210-D4A9-FA40-ABBE-75E4FA51A6A8}">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView zoomScale="140" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A6" zoomScale="140" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="4" max="4" width="15.4609375" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -1118,10 +1127,10 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
         <v>400</v>
@@ -1136,7 +1145,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G3" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H3" s="1">
         <v>3</v>
@@ -1162,13 +1171,13 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="D4" s="1">
         <v>0.01</v>
@@ -1180,7 +1189,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G4" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H4" s="1">
         <v>3</v>
@@ -1206,13 +1215,13 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="D5" s="1">
         <v>0.01</v>
@@ -1224,7 +1233,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G5" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H5" s="1">
         <v>3</v>
@@ -1247,17 +1256,16 @@
       <c r="N5" s="1">
         <v>9.5346210000000001E-2</v>
       </c>
-      <c r="O5" s="1"/>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="D6" s="1">
         <v>0.01</v>
@@ -1269,7 +1277,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G6" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H6" s="1">
         <v>3</v>
@@ -1292,17 +1300,16 @@
       <c r="N6" s="1">
         <v>9.5346210000000001E-2</v>
       </c>
-      <c r="O6" s="1"/>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="D7" s="1">
         <v>0.01</v>
@@ -1314,7 +1321,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G7" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H7" s="1">
         <v>3</v>
@@ -1340,10 +1347,10 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1">
         <v>400</v>
@@ -1358,7 +1365,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G8" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H8" s="1">
         <v>3</v>
@@ -1384,10 +1391,10 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1">
         <v>400</v>
@@ -1402,7 +1409,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G9" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H9" s="1">
         <v>3</v>
@@ -1428,13 +1435,13 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1">
-        <v>110</v>
+        <v>400</v>
       </c>
       <c r="D10" s="1">
         <v>0.01</v>
@@ -1446,7 +1453,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G10" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H10" s="1">
         <v>3</v>
@@ -1471,273 +1478,502 @@
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>400</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="G11" s="1">
+        <v>40</v>
+      </c>
+      <c r="H11" s="1">
+        <v>3</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="1">
+        <v>2</v>
+      </c>
+      <c r="L11" s="1">
+        <v>12</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1711.4</v>
+      </c>
+      <c r="N11" s="1">
+        <v>9.5346210000000001E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
+      <c r="A12" s="1">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>300</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="G12" s="1">
+        <v>40</v>
+      </c>
+      <c r="H12" s="1">
+        <v>3</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="1">
+        <v>2</v>
+      </c>
+      <c r="L12" s="1">
+        <v>12</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1711.4</v>
+      </c>
+      <c r="N12" s="1">
+        <v>9.5346210000000001E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
+      <c r="A13" s="1">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1">
+        <v>300</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="G13" s="1">
+        <v>40</v>
+      </c>
+      <c r="H13" s="1">
+        <v>3</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="1">
+        <v>2</v>
+      </c>
+      <c r="L13" s="1">
+        <v>12</v>
+      </c>
+      <c r="M13" s="1">
+        <v>1711.4</v>
+      </c>
+      <c r="N13" s="1">
+        <v>9.5346210000000001E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
+      <c r="A14" s="1">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1">
+        <v>300</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="G14" s="1">
+        <v>40</v>
+      </c>
+      <c r="H14" s="1">
+        <v>3</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="1">
+        <v>2</v>
+      </c>
+      <c r="L14" s="1">
+        <v>12</v>
+      </c>
+      <c r="M14" s="1">
+        <v>1711.4</v>
+      </c>
+      <c r="N14" s="1">
+        <v>9.5346210000000001E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1">
+      <c r="A15" s="1">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>300</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="G15" s="1">
         <v>40</v>
       </c>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
+      <c r="H15" s="1">
+        <v>3</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="1">
+        <v>2</v>
+      </c>
+      <c r="L15" s="1">
+        <v>12</v>
+      </c>
+      <c r="M15" s="1">
+        <v>1711.4</v>
+      </c>
+      <c r="N15" s="1">
+        <v>9.5346210000000001E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1">
-        <v>30</v>
-      </c>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
+      <c r="A16" s="1">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>300</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="G16" s="1">
+        <v>40</v>
+      </c>
+      <c r="H16" s="1">
+        <v>3</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="1">
+        <v>2</v>
+      </c>
+      <c r="L16" s="1">
+        <v>12</v>
+      </c>
+      <c r="M16" s="1">
+        <v>1711.4</v>
+      </c>
+      <c r="N16" s="1">
+        <v>9.5346210000000001E-2</v>
+      </c>
       <c r="O16" s="1"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1">
-        <v>20</v>
-      </c>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
+      <c r="A17" s="1">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>200</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="G17" s="1">
+        <v>40</v>
+      </c>
+      <c r="H17" s="1">
+        <v>3</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="1">
+        <v>2</v>
+      </c>
+      <c r="L17" s="1">
+        <v>12</v>
+      </c>
+      <c r="M17" s="1">
+        <v>1711.4</v>
+      </c>
+      <c r="N17" s="1">
+        <v>9.5346210000000001E-2</v>
+      </c>
       <c r="O17" s="1"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1">
-        <v>20</v>
-      </c>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
+      <c r="A18" s="1">
+        <v>6</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>300</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="G18" s="1">
+        <v>40</v>
+      </c>
+      <c r="H18" s="1">
+        <v>3</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" s="1">
+        <v>2</v>
+      </c>
+      <c r="L18" s="1">
+        <v>12</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1711.4</v>
+      </c>
+      <c r="N18" s="1">
+        <v>9.5346210000000001E-2</v>
+      </c>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1">
-        <v>20</v>
-      </c>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
+      <c r="A19" s="1">
+        <v>7</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1">
+        <v>400</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="G19" s="1">
+        <v>40</v>
+      </c>
+      <c r="H19" s="1">
+        <v>3</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="1">
+        <v>2</v>
+      </c>
+      <c r="L19" s="1">
+        <v>12</v>
+      </c>
+      <c r="M19" s="1">
+        <v>1711.4</v>
+      </c>
+      <c r="N19" s="1">
+        <v>9.5346210000000001E-2</v>
+      </c>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>33</v>
+      <c r="A20" s="1">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1">
+        <v>400</v>
       </c>
       <c r="D20" s="1">
-        <v>306.10000000000002</v>
+        <v>0.01</v>
       </c>
       <c r="E20" s="1">
-        <v>9.5469999999999999E-2</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F20" s="2">
         <v>1.0000000000000001E-9</v>
       </c>
+      <c r="G20" s="1">
+        <v>40</v>
+      </c>
       <c r="H20" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1">
-        <v>20</v>
-      </c>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" s="1">
+        <v>2</v>
+      </c>
+      <c r="L20" s="1">
+        <v>12</v>
+      </c>
+      <c r="M20" s="1">
+        <v>1711.4</v>
+      </c>
+      <c r="N20" s="1">
+        <v>9.5346210000000001E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1" t="s">
-        <v>35</v>
+      <c r="A21" s="1">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1">
+        <v>9</v>
+      </c>
+      <c r="C21" s="1">
+        <v>110</v>
       </c>
       <c r="D21" s="1">
-        <v>170.2</v>
+        <v>0.01</v>
       </c>
       <c r="E21" s="1">
-        <v>0.17169999999999999</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F21" s="2">
         <v>1.0000000000000001E-9</v>
       </c>
+      <c r="G21" s="1">
+        <v>40</v>
+      </c>
       <c r="H21" s="1">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1">
-        <v>20</v>
-      </c>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="1">
+        <v>2</v>
+      </c>
+      <c r="L21" s="1">
+        <v>12</v>
+      </c>
+      <c r="M21" s="1">
+        <v>1711.4</v>
+      </c>
+      <c r="N21" s="1">
+        <v>9.5346210000000001E-2</v>
+      </c>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1711.4</v>
-      </c>
-      <c r="E22" s="1">
-        <v>2.8379999999999999E-2</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="2">
-        <v>1</v>
-      </c>
-      <c r="H22" s="1">
-        <v>1.875</v>
-      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="1">
-        <v>20</v>
-      </c>
+      <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -1745,9 +1981,7 @@
       <c r="O22" s="1"/>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1755,9 +1989,13 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="J23" s="1">
-        <v>20</v>
-      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
     </row>
     <row r="24" spans="1:15">
       <c r="A24" s="1"/>
@@ -1803,9 +2041,17 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
+      <c r="J26" s="1">
+        <v>40</v>
+      </c>
+      <c r="K26" s="1">
+        <f>J26*2</f>
+        <v>80</v>
+      </c>
+      <c r="L26" s="1">
+        <f>10*J26</f>
+        <v>400</v>
+      </c>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
@@ -1820,12 +2066,347 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
+      <c r="J27" s="1">
+        <v>30</v>
+      </c>
+      <c r="K27" s="1">
+        <f t="shared" ref="K27:K34" si="0">J27*2</f>
+        <v>60</v>
+      </c>
+      <c r="L27" s="1">
+        <f t="shared" ref="L27:L34" si="1">10*J27</f>
+        <v>300</v>
+      </c>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1">
+        <v>20</v>
+      </c>
+      <c r="K28" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="L28" s="1">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1">
+        <v>20</v>
+      </c>
+      <c r="K29" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="L29" s="1">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="M29" s="1"/>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1">
+        <v>20</v>
+      </c>
+      <c r="K30" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="L30" s="1">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="1">
+        <v>306.10000000000002</v>
+      </c>
+      <c r="E31" s="1">
+        <v>9.5469999999999999E-2</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" s="2">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1">
+        <v>20</v>
+      </c>
+      <c r="K31" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="L31" s="1">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="1">
+        <v>170.2</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0.17169999999999999</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G32" s="2">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1">
+        <v>20</v>
+      </c>
+      <c r="K32" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="L32" s="1">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1711.4</v>
+      </c>
+      <c r="E33" s="1">
+        <v>2.8379999999999999E-2</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G33" s="2">
+        <v>1</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1.875</v>
+      </c>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1">
+        <v>20</v>
+      </c>
+      <c r="K33" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="L33" s="1">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="J34" s="1">
+        <v>20</v>
+      </c>
+      <c r="K34" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="L34" s="1">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41" s="1">
+        <v>0</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="A42" s="1">
+        <v>1</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="A43" s="1">
+        <v>2</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44" s="1">
+        <v>3</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
@@ -1839,15 +2420,15 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView zoomScale="136" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:H11"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="4" max="4" width="15.3046875" customWidth="1"/>
-    <col min="5" max="5" width="17.15234375" customWidth="1"/>
-    <col min="7" max="7" width="15.69140625" customWidth="1"/>
-    <col min="8" max="8" width="18.4609375" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2292,13 +2873,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A1CB5C-C75E-D140-AAEC-4E52BCEBAC4C}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView zoomScale="137" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="20.84375" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2430,6 +3011,10 @@
         <f>SUM(D2:D5)</f>
         <v>49002.499980000008</v>
       </c>
+      <c r="E6">
+        <f>SUM(E2:E5)</f>
+        <v>300000</v>
+      </c>
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:7">
@@ -2485,7 +3070,7 @@
     <row r="15" spans="1:7">
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" ht="17">
       <c r="C16" t="s">
         <v>85</v>
       </c>
@@ -2496,7 +3081,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="3:5">
+    <row r="17" spans="3:5" ht="17">
       <c r="C17" t="s">
         <v>89</v>
       </c>
@@ -2507,7 +3092,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="3:5">
+    <row r="18" spans="3:5" ht="17">
       <c r="C18" t="s">
         <v>90</v>
       </c>
@@ -2518,7 +3103,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="3:5">
+    <row r="19" spans="3:5" ht="17">
       <c r="C19" t="s">
         <v>92</v>
       </c>

</xml_diff>

<commit_message>
Added 2050 with pink upgrades
</commit_message>
<xml_diff>
--- a/ThaiModelInput.xlsx
+++ b/ThaiModelInput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williama/Library/Mobile Documents/com~apple~CloudDocs/William's Cloud/Oxford/Small Group Project/Modelling Playground/Thai-PandaPower/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E00033-CA78-6E43-949A-C14ACDD6F9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AF0E89-E9F7-0A4F-AE7F-9628F2F87A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="26200" windowHeight="16640" xr2:uid="{D3764318-3051-D04F-B9CB-11876FC0CA1B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="26200" windowHeight="16640" activeTab="1" xr2:uid="{D3764318-3051-D04F-B9CB-11876FC0CA1B}"/>
   </bookViews>
   <sheets>
     <sheet name="buses" sheetId="1" r:id="rId1"/>
@@ -791,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C88006A-4D90-304B-84D2-9F4A420FC89B}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView zoomScale="138" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1028,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F51210-D4A9-FA40-ABBE-75E4FA51A6A8}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="140" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1101,7 +1101,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G2" s="1">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H2" s="1">
         <v>3</v>
@@ -1145,7 +1145,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G3" s="1">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H3" s="1">
         <v>3</v>
@@ -1189,7 +1189,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G4" s="1">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H4" s="1">
         <v>3</v>
@@ -1233,7 +1233,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G5" s="1">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H5" s="1">
         <v>3</v>
@@ -1277,7 +1277,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G6" s="1">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H6" s="1">
         <v>3</v>
@@ -1321,7 +1321,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G7" s="1">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H7" s="1">
         <v>3</v>
@@ -1365,7 +1365,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G8" s="1">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H8" s="1">
         <v>3</v>
@@ -1409,7 +1409,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G9" s="1">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H9" s="1">
         <v>3</v>
@@ -1453,7 +1453,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G10" s="1">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H10" s="1">
         <v>3</v>
@@ -1497,7 +1497,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G11" s="1">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H11" s="1">
         <v>3</v>
@@ -1541,7 +1541,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G12" s="1">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H12" s="1">
         <v>3</v>
@@ -1585,7 +1585,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G13" s="1">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H13" s="1">
         <v>3</v>
@@ -1629,7 +1629,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G14" s="1">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H14" s="1">
         <v>3</v>
@@ -1673,7 +1673,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G15" s="1">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H15" s="1">
         <v>3</v>
@@ -1717,7 +1717,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G16" s="1">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H16" s="1">
         <v>3</v>
@@ -1762,7 +1762,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G17" s="1">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H17" s="1">
         <v>3</v>
@@ -1807,7 +1807,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G18" s="1">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H18" s="1">
         <v>3</v>
@@ -1851,7 +1851,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G19" s="1">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H19" s="1">
         <v>3</v>
@@ -1895,7 +1895,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G20" s="1">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H20" s="1">
         <v>3</v>
@@ -1939,7 +1939,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="G21" s="1">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H21" s="1">
         <v>3</v>
@@ -2420,7 +2420,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView zoomScale="136" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2874,7 +2874,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="137" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>

</xml_diff>